<commit_message>
add absolute yields for filtering
</commit_message>
<xml_diff>
--- a/data-fix/in.xlsx
+++ b/data-fix/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817CF7D2-0322-4225-AE58-8AB86979EF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11801A07-3C5A-420B-96D3-A225C30E7471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1760,7 +1760,7 @@
   <dimension ref="A1:BO91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add back full data set
</commit_message>
<xml_diff>
--- a/data-fix/in.xlsx
+++ b/data-fix/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11801A07-3C5A-420B-96D3-A225C30E7471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3EF570-18C6-4D7F-8B6D-1C0569A04FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="200">
   <si>
     <t>Austin-Num</t>
   </si>
@@ -621,6 +621,21 @@
   </si>
   <si>
     <t>absolute_yield</t>
+  </si>
+  <si>
+    <t>1-L3</t>
+  </si>
+  <si>
+    <t>3-L16</t>
+  </si>
+  <si>
+    <t>4-L2</t>
+  </si>
+  <si>
+    <t>4-L26</t>
+  </si>
+  <si>
+    <t>DNC</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1475,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3843068" y="638352"/>
+              <a:off x="4464170" y="638352"/>
               <a:ext cx="4572000" cy="2562045"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1757,10 +1772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO91"/>
+  <dimension ref="A1:BK95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95:E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1773,7 +1789,7 @@
     <col min="8" max="62" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>194</v>
       </c>
@@ -1964,7 +1980,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>17.36</v>
       </c>
@@ -2154,12 +2170,8 @@
       <c r="BK2">
         <v>180.23969729999999</v>
       </c>
-      <c r="BO2">
-        <f>IF(C2&lt;0,0,1)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15.67</v>
       </c>
@@ -2349,12 +2361,8 @@
       <c r="BK3">
         <v>179.4490347</v>
       </c>
-      <c r="BO3">
-        <f t="shared" ref="BO3:BO66" si="0">IF(C3&lt;0,0,1)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20.64</v>
       </c>
@@ -2544,12 +2552,8 @@
       <c r="BK4">
         <v>171.9942159</v>
       </c>
-      <c r="BO4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7.62</v>
       </c>
@@ -2739,12 +2743,8 @@
       <c r="BK5">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8.93</v>
       </c>
@@ -2934,12 +2934,8 @@
       <c r="BK6">
         <v>171.9942159</v>
       </c>
-      <c r="BO6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20.38</v>
       </c>
@@ -3129,12 +3125,8 @@
       <c r="BK7">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9.41</v>
       </c>
@@ -3324,12 +3316,8 @@
       <c r="BK8">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9.11</v>
       </c>
@@ -3519,12 +3507,8 @@
       <c r="BK9">
         <v>129.54943950000001</v>
       </c>
-      <c r="BO9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.17</v>
       </c>
@@ -3714,12 +3698,8 @@
       <c r="BK10">
         <v>129.9510459</v>
       </c>
-      <c r="BO10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.2400000000000002</v>
       </c>
@@ -3909,12 +3889,8 @@
       <c r="BK11">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.05</v>
       </c>
@@ -3970,146 +3946,142 @@
         <v>8.3621033257242594</v>
       </c>
       <c r="S12" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="T12">
-        <v>0.15546399999999999</v>
+        <v>999</v>
       </c>
       <c r="U12">
-        <v>-3.7927000000000002E-2</v>
+        <v>999</v>
       </c>
       <c r="V12">
-        <v>-3.7895999999999999E-2</v>
+        <v>999</v>
       </c>
       <c r="W12">
-        <v>-0.43332700000000002</v>
+        <v>999</v>
       </c>
       <c r="X12">
-        <v>0.39064500000000002</v>
+        <v>999</v>
       </c>
       <c r="Y12">
-        <v>-0.17117199999999999</v>
+        <v>999</v>
       </c>
       <c r="Z12">
-        <v>-0.17145299999999999</v>
+        <v>999</v>
       </c>
       <c r="AA12">
-        <v>6.7978999999999998E-2</v>
+        <v>999</v>
       </c>
       <c r="AB12">
-        <v>464.04</v>
+        <v>999</v>
       </c>
       <c r="AC12">
-        <v>158.369</v>
+        <v>999</v>
       </c>
       <c r="AD12">
-        <v>1200.6500000000001</v>
+        <v>999</v>
       </c>
       <c r="AE12">
-        <v>-0.25013999999999997</v>
+        <v>999</v>
       </c>
       <c r="AF12">
-        <v>2.3949999999999999E-2</v>
+        <v>999</v>
       </c>
       <c r="AG12">
-        <v>171.9942159</v>
+        <v>999</v>
       </c>
       <c r="AH12" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="AI12">
-        <v>0.15546399999999999</v>
+        <v>999</v>
       </c>
       <c r="AJ12">
-        <v>-3.7927000000000002E-2</v>
+        <v>999</v>
       </c>
       <c r="AK12">
-        <v>-3.7895999999999999E-2</v>
+        <v>999</v>
       </c>
       <c r="AL12">
-        <v>-0.43332700000000002</v>
+        <v>999</v>
       </c>
       <c r="AM12">
-        <v>0.39064500000000002</v>
+        <v>999</v>
       </c>
       <c r="AN12">
-        <v>-0.17117199999999999</v>
+        <v>999</v>
       </c>
       <c r="AO12">
-        <v>-0.17145299999999999</v>
+        <v>999</v>
       </c>
       <c r="AP12">
-        <v>6.7978999999999998E-2</v>
+        <v>999</v>
       </c>
       <c r="AQ12">
-        <v>464.04</v>
+        <v>999</v>
       </c>
       <c r="AR12">
-        <v>158.369</v>
+        <v>999</v>
       </c>
       <c r="AS12">
-        <v>1200.6500000000001</v>
+        <v>999</v>
       </c>
       <c r="AT12">
-        <v>-0.25013999999999997</v>
+        <v>999</v>
       </c>
       <c r="AU12">
-        <v>2.3949999999999999E-2</v>
+        <v>999</v>
       </c>
       <c r="AV12">
-        <v>171.9942159</v>
+        <v>999</v>
       </c>
       <c r="AW12" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="AX12">
-        <v>0.19575999999999999</v>
+        <v>999</v>
       </c>
       <c r="AY12">
-        <v>-1.7198000000000001E-2</v>
+        <v>999</v>
       </c>
       <c r="AZ12">
-        <v>-2.7101E-2</v>
+        <v>999</v>
       </c>
       <c r="BA12">
-        <v>-0.15559300000000001</v>
+        <v>999</v>
       </c>
       <c r="BB12">
-        <v>0.52158599999999999</v>
+        <v>999</v>
       </c>
       <c r="BC12">
-        <v>-0.184866</v>
+        <v>999</v>
       </c>
       <c r="BD12">
-        <v>-0.150033</v>
+        <v>999</v>
       </c>
       <c r="BE12">
-        <v>-8.6227999999999999E-2</v>
+        <v>999</v>
       </c>
       <c r="BF12">
-        <v>497.02800000000002</v>
+        <v>999</v>
       </c>
       <c r="BG12">
-        <v>58.020899999999997</v>
+        <v>999</v>
       </c>
       <c r="BH12">
-        <v>1117.57</v>
+        <v>999</v>
       </c>
       <c r="BI12">
-        <v>-0.24285999999999999</v>
+        <v>999</v>
       </c>
       <c r="BJ12">
-        <v>-2.409E-2</v>
+        <v>999</v>
       </c>
       <c r="BK12">
-        <v>137.28036270000001</v>
-      </c>
-      <c r="BO12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>999</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>19.73</v>
       </c>
@@ -4299,12 +4271,8 @@
       <c r="BK13">
         <v>137.96434859999999</v>
       </c>
-      <c r="BO13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15.71</v>
       </c>
@@ -4494,12 +4462,8 @@
       <c r="BK14">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13.83</v>
       </c>
@@ -4689,12 +4653,8 @@
       <c r="BK15">
         <v>141.47212949999999</v>
       </c>
-      <c r="BO15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29.55</v>
       </c>
@@ -4884,12 +4844,8 @@
       <c r="BK16">
         <v>137.58156750000001</v>
       </c>
-      <c r="BO16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.99</v>
       </c>
@@ -5079,12 +5035,8 @@
       <c r="BK17">
         <v>107.4987381</v>
       </c>
-      <c r="BO17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.45</v>
       </c>
@@ -5274,12 +5226,8 @@
       <c r="BK18">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.15</v>
       </c>
@@ -5469,12 +5417,8 @@
       <c r="BK19">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.2300000000000004</v>
       </c>
@@ -5664,12 +5608,8 @@
       <c r="BK20">
         <v>117.3192696</v>
       </c>
-      <c r="BO20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.83</v>
       </c>
@@ -5859,12 +5799,8 @@
       <c r="BK21">
         <v>126.6628935</v>
       </c>
-      <c r="BO21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3.12</v>
       </c>
@@ -6054,12 +5990,8 @@
       <c r="BK22">
         <v>117.3192696</v>
       </c>
-      <c r="BO22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8.34</v>
       </c>
@@ -6249,12 +6181,8 @@
       <c r="BK23">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9.25</v>
       </c>
@@ -6444,12 +6372,8 @@
       <c r="BK24">
         <v>114.5896011</v>
       </c>
-      <c r="BO24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7.33</v>
       </c>
@@ -6639,12 +6563,8 @@
       <c r="BK25">
         <v>137.33683859999999</v>
       </c>
-      <c r="BO25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21.76</v>
       </c>
@@ -6834,12 +6754,8 @@
       <c r="BK26">
         <v>175.5835731</v>
       </c>
-      <c r="BO26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14.76</v>
       </c>
@@ -7029,12 +6945,8 @@
       <c r="BK27">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -7224,12 +7136,8 @@
       <c r="BK28">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40.549999999999997</v>
       </c>
@@ -7419,12 +7327,8 @@
       <c r="BK29">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14.75</v>
       </c>
@@ -7614,12 +7518,8 @@
       <c r="BK30">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16.690000000000001</v>
       </c>
@@ -7809,12 +7709,8 @@
       <c r="BK31">
         <v>136.3265475</v>
       </c>
-      <c r="BO31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6.7</v>
       </c>
@@ -8004,12 +7900,8 @@
       <c r="BK32">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.98</v>
       </c>
@@ -8199,12 +8091,8 @@
       <c r="BK33">
         <v>138.3094791</v>
       </c>
-      <c r="BO33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>35.99</v>
       </c>
@@ -8394,12 +8282,8 @@
       <c r="BK34">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8.36</v>
       </c>
@@ -8589,12 +8473,8 @@
       <c r="BK35">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4.3099999999999996</v>
       </c>
@@ -8784,12 +8664,8 @@
       <c r="BK36">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -8979,12 +8855,8 @@
       <c r="BK37">
         <v>114.5896011</v>
       </c>
-      <c r="BO37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15.23</v>
       </c>
@@ -9174,12 +9046,8 @@
       <c r="BK38">
         <v>114.5896011</v>
       </c>
-      <c r="BO38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>16.739999999999998</v>
       </c>
@@ -9369,12 +9237,8 @@
       <c r="BK39">
         <v>113.96209109999999</v>
       </c>
-      <c r="BO39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>28.65</v>
       </c>
@@ -9564,12 +9428,8 @@
       <c r="BK40">
         <v>112.4121414</v>
       </c>
-      <c r="BO40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25.57</v>
       </c>
@@ -9759,12 +9619,8 @@
       <c r="BK41">
         <v>134.8644492</v>
       </c>
-      <c r="BO41">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>24.55</v>
       </c>
@@ -9954,12 +9810,8 @@
       <c r="BK42">
         <v>135.3225315</v>
       </c>
-      <c r="BO42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>14.46</v>
       </c>
@@ -10149,12 +10001,8 @@
       <c r="BK43">
         <v>125.7404538</v>
       </c>
-      <c r="BO43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11.14</v>
       </c>
@@ -10344,12 +10192,8 @@
       <c r="BK44">
         <v>136.29517200000001</v>
       </c>
-      <c r="BO44">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>11.09</v>
       </c>
@@ -10539,12 +10383,8 @@
       <c r="BK45">
         <v>136.29517200000001</v>
       </c>
-      <c r="BO45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>26.65</v>
       </c>
@@ -10734,12 +10574,8 @@
       <c r="BK46">
         <v>129.65611620000001</v>
       </c>
-      <c r="BO46">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>21.11</v>
       </c>
@@ -10929,12 +10765,8 @@
       <c r="BK47">
         <v>137.58156750000001</v>
       </c>
-      <c r="BO47">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>11.9</v>
       </c>
@@ -11124,12 +10956,8 @@
       <c r="BK48">
         <v>137.33683859999999</v>
       </c>
-      <c r="BO48">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="49" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6.59</v>
       </c>
@@ -11319,12 +11147,8 @@
       <c r="BK49">
         <v>129.27961020000001</v>
       </c>
-      <c r="BO49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="50" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -11514,12 +11338,8 @@
       <c r="BK50">
         <v>126.6628935</v>
       </c>
-      <c r="BO50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="51" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>32.4</v>
       </c>
@@ -11709,12 +11529,8 @@
       <c r="BK51">
         <v>135.0527022</v>
       </c>
-      <c r="BO51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="52" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>23.36</v>
       </c>
@@ -11904,12 +11720,8 @@
       <c r="BK52">
         <v>129.54943950000001</v>
       </c>
-      <c r="BO52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="53" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>18.739999999999998</v>
       </c>
@@ -12099,12 +11911,8 @@
       <c r="BK53">
         <v>129.32981100000001</v>
       </c>
-      <c r="BO53">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="54" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9.51</v>
       </c>
@@ -12294,12 +12102,8 @@
       <c r="BK54">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="55" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>20.52</v>
       </c>
@@ -12489,12 +12293,8 @@
       <c r="BK55">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="56" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>35.840000000000003</v>
       </c>
@@ -12684,12 +12484,8 @@
       <c r="BK56">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO56">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="57" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>13.34</v>
       </c>
@@ -12879,12 +12675,8 @@
       <c r="BK57">
         <v>136.3265475</v>
       </c>
-      <c r="BO57">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="58" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6.04</v>
       </c>
@@ -13074,12 +12866,8 @@
       <c r="BK58">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="59" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3.65</v>
       </c>
@@ -13269,12 +13057,8 @@
       <c r="BK59">
         <v>123.01078529999999</v>
       </c>
-      <c r="BO59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="60" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4.7</v>
       </c>
@@ -13464,12 +13248,8 @@
       <c r="BK60">
         <v>167.93422620000001</v>
       </c>
-      <c r="BO60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="61" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -13659,12 +13439,8 @@
       <c r="BK61">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO61">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="62" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>11.22</v>
       </c>
@@ -13854,12 +13630,8 @@
       <c r="BK62">
         <v>123.01078529999999</v>
       </c>
-      <c r="BO62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="63" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>12.96</v>
       </c>
@@ -14049,12 +13821,8 @@
       <c r="BK63">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="64" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -14244,12 +14012,8 @@
       <c r="BK64">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO64">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="65" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>21.15</v>
       </c>
@@ -14439,12 +14203,8 @@
       <c r="BK65">
         <v>140.19200910000001</v>
       </c>
-      <c r="BO65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="66" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.94</v>
       </c>
@@ -14634,12 +14394,8 @@
       <c r="BK66">
         <v>123.01078529999999</v>
       </c>
-      <c r="BO66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="67" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>11.75</v>
       </c>
@@ -14829,12 +14585,8 @@
       <c r="BK67">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO67">
-        <f t="shared" ref="BO67:BO91" si="1">IF(C67&lt;0,0,1)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="68" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -14890,146 +14642,142 @@
         <v>6.5352531359854602</v>
       </c>
       <c r="S68" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="T68">
-        <v>0.22520000000000001</v>
+        <v>999</v>
       </c>
       <c r="U68">
-        <v>-1.8034000000000001E-2</v>
+        <v>999</v>
       </c>
       <c r="V68">
-        <v>-1.6043000000000002E-2</v>
+        <v>999</v>
       </c>
       <c r="W68">
-        <v>-0.315749</v>
+        <v>999</v>
       </c>
       <c r="X68">
-        <v>0.64498999999999995</v>
+        <v>999</v>
       </c>
       <c r="Y68">
-        <v>-0.160193</v>
+        <v>999</v>
       </c>
       <c r="Z68">
-        <v>-0.20486599999999999</v>
+        <v>999</v>
       </c>
       <c r="AA68">
-        <v>-0.14271600000000001</v>
+        <v>999</v>
       </c>
       <c r="AB68">
-        <v>524.827</v>
+        <v>999</v>
       </c>
       <c r="AC68">
-        <v>54.027799999999999</v>
+        <v>999</v>
       </c>
       <c r="AD68">
-        <v>1150.24</v>
+        <v>999</v>
       </c>
       <c r="AE68">
-        <v>-0.23785999999999999</v>
+        <v>999</v>
       </c>
       <c r="AF68">
-        <v>-3.1759999999999997E-2</v>
+        <v>999</v>
       </c>
       <c r="AG68">
-        <v>129.32981100000001</v>
+        <v>999</v>
       </c>
       <c r="AH68" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="AI68">
-        <v>0.22520000000000001</v>
+        <v>999</v>
       </c>
       <c r="AJ68">
-        <v>-1.8034000000000001E-2</v>
+        <v>999</v>
       </c>
       <c r="AK68">
-        <v>-1.6043000000000002E-2</v>
+        <v>999</v>
       </c>
       <c r="AL68">
-        <v>-0.315749</v>
+        <v>999</v>
       </c>
       <c r="AM68">
-        <v>0.64498999999999995</v>
+        <v>999</v>
       </c>
       <c r="AN68">
-        <v>-0.160193</v>
+        <v>999</v>
       </c>
       <c r="AO68">
-        <v>-0.20486599999999999</v>
+        <v>999</v>
       </c>
       <c r="AP68">
-        <v>-0.14271600000000001</v>
+        <v>999</v>
       </c>
       <c r="AQ68">
-        <v>524.827</v>
+        <v>999</v>
       </c>
       <c r="AR68">
-        <v>54.027799999999999</v>
+        <v>999</v>
       </c>
       <c r="AS68">
-        <v>1150.24</v>
+        <v>999</v>
       </c>
       <c r="AT68">
-        <v>-0.23785999999999999</v>
+        <v>999</v>
       </c>
       <c r="AU68">
-        <v>-3.1759999999999997E-2</v>
+        <v>999</v>
       </c>
       <c r="AV68">
-        <v>129.32981100000001</v>
+        <v>999</v>
       </c>
       <c r="AW68" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="AX68">
-        <v>0.22520000000000001</v>
+        <v>999</v>
       </c>
       <c r="AY68">
-        <v>-1.8034000000000001E-2</v>
+        <v>999</v>
       </c>
       <c r="AZ68">
-        <v>-1.6043000000000002E-2</v>
+        <v>999</v>
       </c>
       <c r="BA68">
-        <v>-0.315749</v>
+        <v>999</v>
       </c>
       <c r="BB68">
-        <v>0.64498999999999995</v>
+        <v>999</v>
       </c>
       <c r="BC68">
-        <v>-0.160193</v>
+        <v>999</v>
       </c>
       <c r="BD68">
-        <v>-0.20486599999999999</v>
+        <v>999</v>
       </c>
       <c r="BE68">
-        <v>-0.14271600000000001</v>
+        <v>999</v>
       </c>
       <c r="BF68">
-        <v>524.827</v>
+        <v>999</v>
       </c>
       <c r="BG68">
-        <v>54.027799999999999</v>
+        <v>999</v>
       </c>
       <c r="BH68">
-        <v>1150.24</v>
+        <v>999</v>
       </c>
       <c r="BI68">
-        <v>-0.23785999999999999</v>
+        <v>999</v>
       </c>
       <c r="BJ68">
-        <v>-3.1759999999999997E-2</v>
+        <v>999</v>
       </c>
       <c r="BK68">
-        <v>129.32981100000001</v>
-      </c>
-      <c r="BO68">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>999</v>
       </c>
     </row>
-    <row r="69" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>15.52</v>
       </c>
@@ -15219,12 +14967,8 @@
       <c r="BK69">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="70" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20.76</v>
       </c>
@@ -15414,12 +15158,8 @@
       <c r="BK70">
         <v>138.3094791</v>
       </c>
-      <c r="BO70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="71" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>8.41</v>
       </c>
@@ -15609,12 +15349,8 @@
       <c r="BK71">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO71">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="72" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6.74</v>
       </c>
@@ -15804,12 +15540,8 @@
       <c r="BK72">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO72">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="73" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>15.69</v>
       </c>
@@ -15999,12 +15731,8 @@
       <c r="BK73">
         <v>130.57228079999999</v>
       </c>
-      <c r="BO73">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="74" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.36</v>
       </c>
@@ -16194,12 +15922,8 @@
       <c r="BK74">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO74">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="75" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>10.59</v>
       </c>
@@ -16389,12 +16113,8 @@
       <c r="BK75">
         <v>134.8644492</v>
       </c>
-      <c r="BO75">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="76" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>13.27</v>
       </c>
@@ -16584,12 +16304,8 @@
       <c r="BK76">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO76">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="77" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.9</v>
       </c>
@@ -16779,12 +16495,8 @@
       <c r="BK77">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="78" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.63</v>
       </c>
@@ -16974,12 +16686,8 @@
       <c r="BK78">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="79" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1.83</v>
       </c>
@@ -17169,12 +16877,8 @@
       <c r="BK79">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO79">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="80" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1.18</v>
       </c>
@@ -17364,12 +17068,8 @@
       <c r="BK80">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO80">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="81" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1.31</v>
       </c>
@@ -17559,12 +17259,8 @@
       <c r="BK81">
         <v>137.96434859999999</v>
       </c>
-      <c r="BO81">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="82" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>11.77</v>
       </c>
@@ -17754,12 +17450,8 @@
       <c r="BK82">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO82">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="83" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>8.9600000000000009</v>
       </c>
@@ -17949,12 +17641,8 @@
       <c r="BK83">
         <v>171.9942159</v>
       </c>
-      <c r="BO83">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="84" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>7.43</v>
       </c>
@@ -18144,12 +17832,8 @@
       <c r="BK84">
         <v>129.54943950000001</v>
       </c>
-      <c r="BO84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="85" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>11.79</v>
       </c>
@@ -18339,12 +18023,8 @@
       <c r="BK85">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO85">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="86" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>6.83</v>
       </c>
@@ -18534,12 +18214,8 @@
       <c r="BK86">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO86">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="87" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>14.61</v>
       </c>
@@ -18729,12 +18405,8 @@
       <c r="BK87">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO87">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="88" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>13.18</v>
       </c>
@@ -18924,12 +18596,8 @@
       <c r="BK88">
         <v>137.28036270000001</v>
       </c>
-      <c r="BO88">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="89" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1.18</v>
       </c>
@@ -19119,12 +18787,8 @@
       <c r="BK89">
         <v>107.4987381</v>
       </c>
-      <c r="BO89">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="90" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.18</v>
       </c>
@@ -19314,12 +18978,8 @@
       <c r="BK90">
         <v>107.4987381</v>
       </c>
-      <c r="BO90">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="91" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>6.21</v>
       </c>
@@ -19509,9 +19169,769 @@
       <c r="BK91">
         <v>174.29090249999999</v>
       </c>
-      <c r="BO91">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="92" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0.52</v>
+      </c>
+      <c r="B92">
+        <v>254</v>
+      </c>
+      <c r="C92">
+        <v>-1</v>
+      </c>
+      <c r="D92">
+        <v>0.05</v>
+      </c>
+      <c r="E92">
+        <v>0.17</v>
+      </c>
+      <c r="F92" t="s">
+        <v>198</v>
+      </c>
+      <c r="G92">
+        <v>1.83980270681396</v>
+      </c>
+      <c r="H92">
+        <v>1.84042766769031</v>
+      </c>
+      <c r="I92">
+        <v>1.8399635865962101</v>
+      </c>
+      <c r="J92">
+        <v>105.105863230564</v>
+      </c>
+      <c r="K92">
+        <v>105.08169432069499</v>
+      </c>
+      <c r="L92">
+        <v>103.882760517318</v>
+      </c>
+      <c r="M92">
+        <v>66.088155180790295</v>
+      </c>
+      <c r="N92">
+        <v>29.070629997844499</v>
+      </c>
+      <c r="O92">
+        <v>41.5</v>
+      </c>
+      <c r="P92">
+        <v>8.9384126354144495</v>
+      </c>
+      <c r="Q92">
+        <v>5.6573312499376804</v>
+      </c>
+      <c r="R92">
+        <v>7.6087912524532104</v>
+      </c>
+      <c r="S92" t="s">
+        <v>165</v>
+      </c>
+      <c r="T92">
+        <v>0.22301699999999999</v>
+      </c>
+      <c r="U92">
+        <v>-1.1913E-2</v>
+      </c>
+      <c r="V92">
+        <v>-4.6870000000000002E-3</v>
+      </c>
+      <c r="W92">
+        <v>-0.14432</v>
+      </c>
+      <c r="X92">
+        <v>0.46884199999999998</v>
+      </c>
+      <c r="Y92">
+        <v>-0.13273799999999999</v>
+      </c>
+      <c r="Z92">
+        <v>-0.147151</v>
+      </c>
+      <c r="AA92">
+        <v>-4.0252000000000003E-2</v>
+      </c>
+      <c r="AB92">
+        <v>491.35899999999998</v>
+      </c>
+      <c r="AC92">
+        <v>51.790700000000001</v>
+      </c>
+      <c r="AD92">
+        <v>1117.94</v>
+      </c>
+      <c r="AE92">
+        <v>-0.25564999999999999</v>
+      </c>
+      <c r="AF92">
+        <v>-5.527E-2</v>
+      </c>
+      <c r="AG92">
+        <v>125.7404538</v>
+      </c>
+      <c r="AH92" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI92">
+        <v>0.22301699999999999</v>
+      </c>
+      <c r="AJ92">
+        <v>-1.1913E-2</v>
+      </c>
+      <c r="AK92">
+        <v>-4.6870000000000002E-3</v>
+      </c>
+      <c r="AL92">
+        <v>-0.14432</v>
+      </c>
+      <c r="AM92">
+        <v>0.46884199999999998</v>
+      </c>
+      <c r="AN92">
+        <v>-0.13273799999999999</v>
+      </c>
+      <c r="AO92">
+        <v>-0.147151</v>
+      </c>
+      <c r="AP92">
+        <v>-4.0252000000000003E-2</v>
+      </c>
+      <c r="AQ92">
+        <v>491.35899999999998</v>
+      </c>
+      <c r="AR92">
+        <v>51.790700000000001</v>
+      </c>
+      <c r="AS92">
+        <v>1117.94</v>
+      </c>
+      <c r="AT92">
+        <v>-0.25564999999999999</v>
+      </c>
+      <c r="AU92">
+        <v>-5.527E-2</v>
+      </c>
+      <c r="AV92">
+        <v>125.7404538</v>
+      </c>
+      <c r="AW92" t="s">
+        <v>163</v>
+      </c>
+      <c r="AX92">
+        <v>0.210537</v>
+      </c>
+      <c r="AY92">
+        <v>-0.18282599999999999</v>
+      </c>
+      <c r="AZ92">
+        <v>-2.5245E-2</v>
+      </c>
+      <c r="BA92">
+        <v>-8.1609999999999999E-3</v>
+      </c>
+      <c r="BB92">
+        <v>0.50115699999999996</v>
+      </c>
+      <c r="BC92">
+        <v>-0.142571</v>
+      </c>
+      <c r="BD92">
+        <v>-0.15087999999999999</v>
+      </c>
+      <c r="BE92">
+        <v>-0.130694</v>
+      </c>
+      <c r="BF92">
+        <v>524.41399999999999</v>
+      </c>
+      <c r="BG92">
+        <v>65.549800000000005</v>
+      </c>
+      <c r="BH92">
+        <v>1095.94</v>
+      </c>
+      <c r="BI92">
+        <v>-0.20849000000000001</v>
+      </c>
+      <c r="BJ92">
+        <v>-2.1530000000000001E-2</v>
+      </c>
+      <c r="BK92">
+        <v>117.3192696</v>
+      </c>
+    </row>
+    <row r="93" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B93">
+        <v>18</v>
+      </c>
+      <c r="C93">
+        <v>-0.99</v>
+      </c>
+      <c r="D93">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E93">
+        <v>0.25</v>
+      </c>
+      <c r="F93" t="s">
+        <v>197</v>
+      </c>
+      <c r="G93">
+        <v>1.8541372656845001</v>
+      </c>
+      <c r="H93">
+        <v>1.8532538951800399</v>
+      </c>
+      <c r="I93">
+        <v>1.8536437090228499</v>
+      </c>
+      <c r="J93">
+        <v>105.54222389781</v>
+      </c>
+      <c r="K93">
+        <v>105.381185444132</v>
+      </c>
+      <c r="L93">
+        <v>105.977217511124</v>
+      </c>
+      <c r="M93">
+        <v>66.919614905551597</v>
+      </c>
+      <c r="N93">
+        <v>29.560624386951801</v>
+      </c>
+      <c r="O93">
+        <v>52.4</v>
+      </c>
+      <c r="P93">
+        <v>7.0951754566917398</v>
+      </c>
+      <c r="Q93">
+        <v>5.0637655464697904</v>
+      </c>
+      <c r="R93">
+        <v>7.50501181044506</v>
+      </c>
+      <c r="S93" t="s">
+        <v>159</v>
+      </c>
+      <c r="T93">
+        <v>0.211315</v>
+      </c>
+      <c r="U93">
+        <v>-1.2241999999999999E-2</v>
+      </c>
+      <c r="V93">
+        <v>-2.5786E-2</v>
+      </c>
+      <c r="W93">
+        <v>-0.17399600000000001</v>
+      </c>
+      <c r="X93">
+        <v>0.42102099999999998</v>
+      </c>
+      <c r="Y93">
+        <v>-0.14943100000000001</v>
+      </c>
+      <c r="Z93">
+        <v>-0.14927199999999999</v>
+      </c>
+      <c r="AA93">
+        <v>0.32790900000000001</v>
+      </c>
+      <c r="AB93">
+        <v>495.55799999999999</v>
+      </c>
+      <c r="AC93">
+        <v>28.220099999999999</v>
+      </c>
+      <c r="AD93">
+        <v>1160.07</v>
+      </c>
+      <c r="AE93">
+        <v>-0.24703</v>
+      </c>
+      <c r="AF93">
+        <v>-3.9059999999999997E-2</v>
+      </c>
+      <c r="AG93">
+        <v>130.50325470000001</v>
+      </c>
+      <c r="AH93" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI93">
+        <v>0.19575999999999999</v>
+      </c>
+      <c r="AJ93">
+        <v>-1.7198000000000001E-2</v>
+      </c>
+      <c r="AK93">
+        <v>-2.7101E-2</v>
+      </c>
+      <c r="AL93">
+        <v>-0.15559300000000001</v>
+      </c>
+      <c r="AM93">
+        <v>0.52158599999999999</v>
+      </c>
+      <c r="AN93">
+        <v>-0.184866</v>
+      </c>
+      <c r="AO93">
+        <v>-0.150033</v>
+      </c>
+      <c r="AP93">
+        <v>-8.6227999999999999E-2</v>
+      </c>
+      <c r="AQ93">
+        <v>497.02800000000002</v>
+      </c>
+      <c r="AR93">
+        <v>58.020899999999997</v>
+      </c>
+      <c r="AS93">
+        <v>1117.57</v>
+      </c>
+      <c r="AT93">
+        <v>-0.24285999999999999</v>
+      </c>
+      <c r="AU93">
+        <v>-2.409E-2</v>
+      </c>
+      <c r="AV93">
+        <v>137.28036270000001</v>
+      </c>
+      <c r="AW93" t="s">
+        <v>154</v>
+      </c>
+      <c r="AX93">
+        <v>0.19575999999999999</v>
+      </c>
+      <c r="AY93">
+        <v>-1.7198000000000001E-2</v>
+      </c>
+      <c r="AZ93">
+        <v>-2.7101E-2</v>
+      </c>
+      <c r="BA93">
+        <v>-0.15559300000000001</v>
+      </c>
+      <c r="BB93">
+        <v>0.52158599999999999</v>
+      </c>
+      <c r="BC93">
+        <v>-0.184866</v>
+      </c>
+      <c r="BD93">
+        <v>-0.150033</v>
+      </c>
+      <c r="BE93">
+        <v>-8.6227999999999999E-2</v>
+      </c>
+      <c r="BF93">
+        <v>497.02800000000002</v>
+      </c>
+      <c r="BG93">
+        <v>58.020899999999997</v>
+      </c>
+      <c r="BH93">
+        <v>1117.57</v>
+      </c>
+      <c r="BI93">
+        <v>-0.24285999999999999</v>
+      </c>
+      <c r="BJ93">
+        <v>-2.409E-2</v>
+      </c>
+      <c r="BK93">
+        <v>137.28036270000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1.36</v>
+      </c>
+      <c r="B94">
+        <v>263</v>
+      </c>
+      <c r="C94">
+        <v>-0.77</v>
+      </c>
+      <c r="D94">
+        <v>0.09</v>
+      </c>
+      <c r="E94">
+        <v>0.13</v>
+      </c>
+      <c r="F94" t="s">
+        <v>196</v>
+      </c>
+      <c r="G94">
+        <v>1.8430881693505601</v>
+      </c>
+      <c r="H94">
+        <v>1.8412392565878</v>
+      </c>
+      <c r="I94">
+        <v>1.8433268836535699</v>
+      </c>
+      <c r="J94">
+        <v>99.821448293993797</v>
+      </c>
+      <c r="K94">
+        <v>104.82983567753</v>
+      </c>
+      <c r="L94">
+        <v>104.26991269037499</v>
+      </c>
+      <c r="M94">
+        <v>64.601544509877797</v>
+      </c>
+      <c r="N94">
+        <v>28.4617199449178</v>
+      </c>
+      <c r="O94">
+        <v>40.5</v>
+      </c>
+      <c r="P94">
+        <v>7.6318996147509397</v>
+      </c>
+      <c r="Q94">
+        <v>4.2587521318263901</v>
+      </c>
+      <c r="R94">
+        <v>6.4121844428076802</v>
+      </c>
+      <c r="S94" t="s">
+        <v>170</v>
+      </c>
+      <c r="T94">
+        <v>0.15173600000000001</v>
+      </c>
+      <c r="U94">
+        <v>-3.4506000000000002E-2</v>
+      </c>
+      <c r="V94">
+        <v>-3.4562000000000002E-2</v>
+      </c>
+      <c r="W94">
+        <v>-0.12188300000000001</v>
+      </c>
+      <c r="X94">
+        <v>0.41831699999999999</v>
+      </c>
+      <c r="Y94">
+        <v>-0.151834</v>
+      </c>
+      <c r="Z94">
+        <v>-0.15231600000000001</v>
+      </c>
+      <c r="AA94">
+        <v>-8.7807999999999997E-2</v>
+      </c>
+      <c r="AB94">
+        <v>465.73599999999999</v>
+      </c>
+      <c r="AC94">
+        <v>161.79400000000001</v>
+      </c>
+      <c r="AD94">
+        <v>1249.75</v>
+      </c>
+      <c r="AE94">
+        <v>-0.23638000000000001</v>
+      </c>
+      <c r="AF94">
+        <v>-1.5970000000000002E-2</v>
+      </c>
+      <c r="AG94">
+        <v>138.3094791</v>
+      </c>
+      <c r="AH94" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI94">
+        <v>0.19575999999999999</v>
+      </c>
+      <c r="AJ94">
+        <v>-1.7198000000000001E-2</v>
+      </c>
+      <c r="AK94">
+        <v>-2.7101E-2</v>
+      </c>
+      <c r="AL94">
+        <v>-0.15559300000000001</v>
+      </c>
+      <c r="AM94">
+        <v>0.52158599999999999</v>
+      </c>
+      <c r="AN94">
+        <v>-0.184866</v>
+      </c>
+      <c r="AO94">
+        <v>-0.150033</v>
+      </c>
+      <c r="AP94">
+        <v>-8.6227999999999999E-2</v>
+      </c>
+      <c r="AQ94">
+        <v>497.02800000000002</v>
+      </c>
+      <c r="AR94">
+        <v>58.020899999999997</v>
+      </c>
+      <c r="AS94">
+        <v>1117.57</v>
+      </c>
+      <c r="AT94">
+        <v>-0.24285999999999999</v>
+      </c>
+      <c r="AU94">
+        <v>-2.409E-2</v>
+      </c>
+      <c r="AV94">
+        <v>137.28036270000001</v>
+      </c>
+      <c r="AW94" t="s">
+        <v>154</v>
+      </c>
+      <c r="AX94">
+        <v>0.19575999999999999</v>
+      </c>
+      <c r="AY94">
+        <v>-1.7198000000000001E-2</v>
+      </c>
+      <c r="AZ94">
+        <v>-2.7101E-2</v>
+      </c>
+      <c r="BA94">
+        <v>-0.15559300000000001</v>
+      </c>
+      <c r="BB94">
+        <v>0.52158599999999999</v>
+      </c>
+      <c r="BC94">
+        <v>-0.184866</v>
+      </c>
+      <c r="BD94">
+        <v>-0.150033</v>
+      </c>
+      <c r="BE94">
+        <v>-8.6227999999999999E-2</v>
+      </c>
+      <c r="BF94">
+        <v>497.02800000000002</v>
+      </c>
+      <c r="BG94">
+        <v>58.020899999999997</v>
+      </c>
+      <c r="BH94">
+        <v>1117.57</v>
+      </c>
+      <c r="BI94">
+        <v>-0.24285999999999999</v>
+      </c>
+      <c r="BJ94">
+        <v>-2.409E-2</v>
+      </c>
+      <c r="BK94">
+        <v>137.28036270000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A95">
         <v>0</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>195</v>
+      </c>
+      <c r="G95">
+        <v>1.90599711437347</v>
+      </c>
+      <c r="H95">
+        <v>1.90496981603383</v>
+      </c>
+      <c r="I95">
+        <v>1.87327654125065</v>
+      </c>
+      <c r="J95">
+        <v>115.66327392451601</v>
+      </c>
+      <c r="K95">
+        <v>107.476125313289</v>
+      </c>
+      <c r="L95">
+        <v>105.618954714742</v>
+      </c>
+      <c r="M95">
+        <v>70.538991746262894</v>
+      </c>
+      <c r="N95">
+        <v>31.539631237989401</v>
+      </c>
+      <c r="O95">
+        <v>54.3</v>
+      </c>
+      <c r="P95">
+        <v>6.4928007774058498</v>
+      </c>
+      <c r="Q95">
+        <v>4.0312885399118201</v>
+      </c>
+      <c r="R95">
+        <v>6.2239199054111198</v>
+      </c>
+      <c r="S95" t="s">
+        <v>150</v>
+      </c>
+      <c r="T95">
+        <v>0.15546399999999999</v>
+      </c>
+      <c r="U95">
+        <v>-3.7927000000000002E-2</v>
+      </c>
+      <c r="V95">
+        <v>-3.7895999999999999E-2</v>
+      </c>
+      <c r="W95">
+        <v>-0.43332700000000002</v>
+      </c>
+      <c r="X95">
+        <v>0.39064500000000002</v>
+      </c>
+      <c r="Y95">
+        <v>-0.17117199999999999</v>
+      </c>
+      <c r="Z95">
+        <v>-0.17145299999999999</v>
+      </c>
+      <c r="AA95">
+        <v>6.7978999999999998E-2</v>
+      </c>
+      <c r="AB95">
+        <v>464.04</v>
+      </c>
+      <c r="AC95">
+        <v>158.369</v>
+      </c>
+      <c r="AD95">
+        <v>1200.6500000000001</v>
+      </c>
+      <c r="AE95">
+        <v>-0.25013999999999997</v>
+      </c>
+      <c r="AF95">
+        <v>2.3949999999999999E-2</v>
+      </c>
+      <c r="AG95">
+        <v>171.9942159</v>
+      </c>
+      <c r="AH95" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI95">
+        <v>0.15546399999999999</v>
+      </c>
+      <c r="AJ95">
+        <v>-3.7927000000000002E-2</v>
+      </c>
+      <c r="AK95">
+        <v>-3.7895999999999999E-2</v>
+      </c>
+      <c r="AL95">
+        <v>-0.43332700000000002</v>
+      </c>
+      <c r="AM95">
+        <v>0.39064500000000002</v>
+      </c>
+      <c r="AN95">
+        <v>-0.17117199999999999</v>
+      </c>
+      <c r="AO95">
+        <v>-0.17145299999999999</v>
+      </c>
+      <c r="AP95">
+        <v>6.7978999999999998E-2</v>
+      </c>
+      <c r="AQ95">
+        <v>464.04</v>
+      </c>
+      <c r="AR95">
+        <v>158.369</v>
+      </c>
+      <c r="AS95">
+        <v>1200.6500000000001</v>
+      </c>
+      <c r="AT95">
+        <v>-0.25013999999999997</v>
+      </c>
+      <c r="AU95">
+        <v>2.3949999999999999E-2</v>
+      </c>
+      <c r="AV95">
+        <v>171.9942159</v>
+      </c>
+      <c r="AW95" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX95">
+        <v>0.112469</v>
+      </c>
+      <c r="AY95">
+        <v>-3.7032000000000002E-2</v>
+      </c>
+      <c r="AZ95">
+        <v>-3.7026999999999997E-2</v>
+      </c>
+      <c r="BA95">
+        <v>-0.218081</v>
+      </c>
+      <c r="BB95">
+        <v>0.49265900000000001</v>
+      </c>
+      <c r="BC95">
+        <v>-0.17632500000000001</v>
+      </c>
+      <c r="BD95">
+        <v>-0.17619299999999999</v>
+      </c>
+      <c r="BE95">
+        <v>-0.13664899999999999</v>
+      </c>
+      <c r="BF95">
+        <v>533.56399999999996</v>
+      </c>
+      <c r="BG95">
+        <v>189.25299999999999</v>
+      </c>
+      <c r="BH95">
+        <v>1297.81</v>
+      </c>
+      <c r="BI95">
+        <v>-0.25402000000000002</v>
+      </c>
+      <c r="BJ95">
+        <v>3.3210000000000003E-2</v>
+      </c>
+      <c r="BK95">
+        <v>180.23969729999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new new best result
</commit_message>
<xml_diff>
--- a/data-fix/in.xlsx
+++ b/data-fix/in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A638FDA5-5363-4AA5-A04F-BA3E7186C08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6347EE40-BDF6-499D-9D0C-11313F399EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1775,8 +1775,8 @@
   <dimension ref="A1:BK95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>